<commit_message>
author error handled by error page
</commit_message>
<xml_diff>
--- a/mylibrary.xlsx
+++ b/mylibrary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\munozm\Desktop\imreading\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E6F22A-FB96-489C-9B2A-4C5C63C4A549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B297729-0633-4A59-9C34-5CA69CC3F702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1800" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="25800" windowHeight="10140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SHELVES" sheetId="2" r:id="rId1"/>
@@ -19,11 +19,12 @@
     <sheet name="SHELVED_BOOKS" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="303">
   <si>
     <t>The Dutch House</t>
   </si>
@@ -694,111 +695,19 @@
     <t>null</t>
   </si>
   <si>
-    <t>*A story about forgiving the past.*
-I do not believe an audiobook was the best choice for this book. Though Tom Hanks as narrator is superb!
-The timelines jump so much, I felt slightly dizzy sometimes trying to wrap my brains around the narration. I believe in the book, I would have gotten those empty spaces to help. But here, there was a second between scene, making it seem it was still the same scene, just to fall into the actual one like jumping through dream scenes. It was wild.
-The story itself was nice, but it is more like an autobiography. For those complaining of no plot, you missed the story. The plot was always Daniel’s dreams, which all begun with his father and the Dutch House. The characters were good, but not amazing. The prose, though, the prose! The writing style is breathtaking, and I can see why so many people love this book. I can savor each word, and I am sad the library did not have the book available for me to read along.
-The plot progressed in random jumps... chapter ends, chapter start with first few lines with a new event. For a while I had the feeling Maeve and Celeste were in love before Maeve pushed her into Daniel. In the end, when all comes in full circle, it is truly a story about forgiveness at its very core. About how no one is exempt from mistakes and tragedy and that should not hold us from enjoying life, the way May always did. It feels May was the embodiment of the resolution. A clean slate for the family. Enjoying life, and not caring about the past, but about moving forward.</t>
-  </si>
-  <si>
     <t>🙂</t>
   </si>
   <si>
     <t>🤨</t>
   </si>
   <si>
-    <t>Someone knew about the coins… that doesn't make sense.</t>
-  </si>
-  <si>
-    <t>"Fossils put my memories into perspective. They tell me, I too, with my centuries of memory, am no more than the faintest shadow on the landscape of time."</t>
-  </si>
-  <si>
     <t>😍</t>
   </si>
   <si>
-    <t xml:space="preserve"> Now this is the kind of story that drags me in!</t>
-  </si>
-  <si>
-    <t>I love this style so so so much!</t>
-  </si>
-  <si>
     <t>That was intense! I was feeling so disgusted 🤢</t>
   </si>
   <si>
-    <t>This is about embracing the now. WOW</t>
-  </si>
-  <si>
-    <t>This is my kind of book. A mix of Historical fiction and Scifi. These were amazing characters. Incredible narration. Flowing prose, just so gentle and dreamy.
-The reason for the memories was unexpected and certainly the end, and what they did with Halley’s eggs was something I was not expecting. Which is something not all books can give me lately. I love love loved this book so much. The adventures, the journey, I felt like I lived them myself. The beauty of the now in contrast to the memories. Memories are but a tool in the end, not something to make you feel despair or rage, or joy. But a tool to help you survive in the future and help you realize the beauty of the now.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19/2 Starts with Sid and his partner Ian solving a muddler crime. Sid sounds old, tired from jokes and very empathic. Same night, the murder of one of the clones.
-20/2 kids 8 &amp; 6. Small house to big house. Jacinta a health hobbyist.
-- Zone room?
-- Economy : bioil
-Berlin seems to be the capital government. One of the clones lives around Jupiter, another on earth. The Agustine family on st libra. The clone dead is probably a Jupiter one. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vance, typical male arch. Berlin investigator. Involved in previous case. Seems like a good guy. 
-Zanth? Aliens? 
-Angela - one in ten : one bio year every ten, slow aging. Which means she's 200 years old.  That means they could live for thousands of years under natural circumstances. </t>
-  </si>
-  <si>
-    <t>14 victims 20 years ago</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Clayton 2North and Rebka
-Tuesday 15 Jan 2143 : previous victim, Bartram North and family</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> still busy with the investigation. Lots of details… reminds me why I don’t like detective movies. But curious about where it will lead. I want them to start the alien expedition already!</t>
-  </si>
-  <si>
-    <t>It starts slooowww, the whole first part is the MC in the maternity room. The dialog style is annoying. I keep having to go back to reread it after I know who spoke and if out loud or in thoughts.
-The concept itself makes me keep reading to see where it goes.</t>
-  </si>
-  <si>
-    <t>That was very very very unexpected. Nothing against it. It is lovely. But I have the feeling most Historical Fiction books I've been reading lately are all homosexual couples... I kind of like daydreaming with straights... since I am... happy for the characters but leaves me with no daydreaming topic hahaha</t>
-  </si>
-  <si>
-    <t>interesting plot, lovely main female character. 
-Male lead is a bit annoying... too fast too hard too cheesy and puukey. 
-MC is confused. Does he die for helping her or not???? (look for the quotes)
-FC being bi felt very random and forced, as if to market the book as diverse. I hate that. I enjoy diversity where diversity fits, where it fits the story. Else, why bother mentioning it? Characters just like us can have their own inner secret world. “Hey, here is a love story of a girl and an alien, who is male, but don’t hate me for liking heterosexual romance! She’s bi!”</t>
-  </si>
-  <si>
-    <t>ok.... now I am reading out of curiosity. But it is a bit annoying to read. The “big guys” sound all retarded, believing every bad lie from the ML. The "I'm so inclusive, even my aliens are nonbinary" in-your-face thing is becoming too much. And I did not miss all the melodramatic and raging teen hormones... I think this will be my last YA. I'm too old for this</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	This is the most cheesy, over the top teenage love, hyper inclusivity thing I've ever read.
-It started promising. But it became so much I could not handle it. It took me a few days to finish the last 50 pages... but I needed to finish it out of curiosity. The Allister part was what I was hoping for. It felt I was reading a romance fanfic with K-pop and aliens. </t>
-  </si>
-  <si>
     <t>🤮</t>
-  </si>
-  <si>
-    <t>Main character is annoying. The whole way. We should could how many times the word Asshole appears in the book.
-What kept me reading is the theme.
-A lot of things seem to happen at random, so much in one go, but it is entertaining. It plays like  a movie in my head. Or a mini series considering the length.
-what a crazy rideeeeeeeee</t>
-  </si>
-  <si>
-    <t>It is sooo weird and condescending with criticizing every single element of modern society. Even things that should be logical. If they study life on other planets, they should know all life is different. This shows the "aliens" as stupid ATM... and that annoys me. But I am intrigued. The writing is good. It is just the character... so annoying.</t>
-  </si>
-  <si>
-    <t>It's getting a bit better.</t>
-  </si>
-  <si>
-    <t>Entertaining but not amazing. Like TV in a tired night.</t>
-  </si>
-  <si>
-    <t>Wow. Loved the narration. Was sad for some characters, :( was sad for humanity. There is something about end of times books that just triggers me to embrace this moment because one day we will be gone.</t>
-  </si>
-  <si>
-    <t>Got too technical and no plot... I could not read naother word about the secret weapons program.</t>
-  </si>
-  <si>
-    <t>Nop. not going to finish it. It is so much science and so little story... I am sure that without the science, it would have been one of his many short stories.</t>
   </si>
   <si>
     <t>Thought I might not like it. Started it years ago. No. But now, it was what I was looking for. Sometimes it's not the book, it's the timing.</t>
@@ -948,6 +857,93 @@
   </si>
   <si>
     <t>Shin is the sea god, this was so good! I had to stop working and close my eyes to savor the last hour.</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;&lt;b&gt;A story about forgiving the past.&lt;/b&gt;&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;&lt;b&gt;&lt;br&gt;&lt;/b&gt;&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;I do not believe an audiobook was the best choice for this book. Though Tom Hanks as narrator is superb!&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;The timelines jump so much, I felt slightly dizzy sometimes trying to wrap my brains around the narration. I believe in the book, I would have gotten those empty spaces to help. But here, there was a second between scene, making it seem it was still the same scene, just to fall into the actual one like jumping through dream scenes. It was wild.&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;The story itself was nice, but it is more like an autobiography. For those complaining of no plot, you missed the story. The plot was always Daniel’s dreams, which all begun with his father and the Dutch House. The characters were good, but not amazing. The prose, though, the prose! The writing style is breathtaking, and I can see why so many people love this book. I can savor each word, and I am sad the library did not have the book available for me to read along.&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;The plot progressed in random jumps... chapter ends, chapter start with first few lines with a new event. For a while I had the feeling Maeve and Celeste were in love before Maeve pushed her into Daniel. In the end, when all comes in full circle, it is truly a story about forgiveness at its very core. About how no one is exempt from mistakes and tragedy and that should not hold us from enjoying life, the way May always did. It feels May was the embodiment of the resolution. A clean slate for the family. Enjoying life, and not caring about the past, but about moving forward.&lt;/span&gt;&lt;/div&gt;&lt;/div&gt;&lt;div&gt;&lt;br&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;&amp;nbsp;Now this is the kind of story that drags me in!&lt;/span&gt;&lt;/div&gt;&lt;/div&gt;&lt;div&gt;&lt;br&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;I love this style so so so much!&lt;/span&gt;&lt;/div&gt;&lt;/div&gt;&lt;div&gt;&lt;br&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;Someone knew about the coins… that doesn't make sense.&lt;/span&gt;&lt;/div&gt;&lt;/div&gt;&lt;div&gt;&lt;br&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;&lt;h3&gt;&lt;i&gt;"Fossils put my memories into perspective. They tell me, I too, with my centuries of memory, am no more than the faintest shadow on the landscape of time."&lt;/i&gt;&lt;/h3&gt;&lt;/span&gt;&lt;/div&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;This is about embracing the now. WOW&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;This is my kind of book.&lt;b&gt; A mix of Historical fiction and Scifi.&lt;/b&gt; These were amazing characters. Incredible narration. Flowing prose, just so gentle and dreamy.&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;The reason for the memories was unexpected and certainly the end, and what they did with Halley’s eggs was something I was not expecting. Which is something not all books can give me lately. I love love loved this book so much. The adventures, the journey, I felt like I lived them myself. The beauty of the now in contrast to the memories. Memories are but a tool in the end, not something to make you feel despair or rage, or joy. But a tool to help you survive in the future and help you realize the beauty of the now.&lt;/span&gt;&lt;/div&gt;&lt;/div&gt;&lt;div&gt;&lt;br&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>💬</t>
+  </si>
+  <si>
+    <t>🤢</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;div&gt;&lt;ul&gt;&lt;li&gt;&lt;span style="font-size: 12px;"&gt;19/2 Starts with Sid and his partner Ian solving a murder crime. Sid sounds old, tired from jokes and very empathic. Same night, the murder of one of the clones.&lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="font-size: 12px;"&gt;20/2 kids 8 &amp;amp; 6. Small house to big house. Jacinta, a health hobbyist.&lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="font-size: 12px;"&gt;-Zone room?&lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="font-size: 12px;"&gt;Economy : bio-oil&lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="font-size: 12px;"&gt;Berlin seems to be the capital of government. One of the clones lives around Jupiter, another on earth. The Agustine family on st libra. The clone dead is probably a Jupiter one.&amp;nbsp;&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;&lt;/div&gt;	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;div&gt;&lt;div&gt;&lt;ul&gt;&lt;li&gt;&lt;span style="font-size: 12px;"&gt;&lt;b&gt;Vance&lt;/b&gt;, typical male arch. Berlin investigator. Involved in previous case. Seems like a good guy.&amp;nbsp;&lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="font-size: 12px;"&gt;Zanth? Aliens?&amp;nbsp;&lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="font-size: 12px;"&gt;&lt;b&gt;Angela &lt;/b&gt;- one in ten : one bio year every ten, slow aging. Which means she's 200 years old.&amp;nbsp; That means they could live for thousands of years under natural circumstances.&amp;nbsp;&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;&lt;/div&gt;&lt;/div&gt;&lt;div&gt;&lt;br&gt;&lt;/div&gt;	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;14 victims 20 years ago from same kind of death, witnessed by Angelica&lt;/span&gt;&lt;/div&gt;&lt;/div&gt;&lt;div&gt;&lt;br&gt;&lt;/div&gt;	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;Clayton 2North and Rebka&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;Tuesday 15 Jan 2143 : previous victim, Bartram North and family&lt;/span&gt;&lt;/div&gt;&lt;/div&gt;&lt;div&gt;&lt;br&gt;&lt;/div&gt;	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;still busy with the investigation. Lots of details… reminds me why I don’t like detective movies. But curious about where it will lead. I want them to start the alien expedition already!&lt;/span&gt;&lt;/div&gt;&lt;/div&gt;&lt;div&gt;&lt;br&gt;&lt;/div&gt;	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;div&gt;&lt;span style="font-size: 12px;"&gt;So there is a fake North replacing the dead North. But why dump the body instead of burning? It sounds too stupid and on purpose. And I just read the back of the book... Sounds like horror scifi, my last fav. sub genre.&amp;nbsp;&lt;/span&gt;&lt;br&gt;&lt;/div&gt;	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;ok.... now I am reading out of curiosity. But it is a bit annoying to read. The “big guys” sound all retarded, believing every bad lie from the ML. The &lt;i&gt;"I'm so inclusive, even my aliens are nonbinary"&lt;/i&gt; in-your-face thing is becoming too much. And I did not miss all the melodramatic and raging teen hormones... I think this will be my last YA. &lt;b&gt;I'm too old for this.&lt;/b&gt;&lt;/span&gt;&lt;/div&gt;&lt;/div&gt;	</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;This is the most cheesy, over the top teenage love, hyper inclusivity thing I've ever read.&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;It started promising. But it became so much I could not handle it. It took me a few days to finish the last 50 pages... but I needed to finish it out of curiosity.&amp;nbsp;&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;The Allister part was what I was hoping for. It felt I was reading a romance fanfic with K-pop and aliens.&amp;nbsp;&lt;/span&gt;&lt;/div&gt;&lt;/div&gt;&lt;div&gt;&lt;br&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;Interesting plot, lovely main female character.&amp;nbsp;&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;Male lead is a bit annoying... too fast, too hard, too cheesy and pukey.&amp;nbsp;&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;MC is confused. Does he die for helping her or not???? (look for the quotes)&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;FC being bi felt very random and forced, as if to market the book as diverse. I hate that. I enjoy diversity where diversity fits, where it fits the story. Else, why bother mentioning it? Characters just like us can have their own inner secret world.&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;&lt;i&gt;“Hey, here is a love story of a girl and an alien, who is male, but don’t hate me for liking heterosexual romance! She’s bi!”&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;/div&gt;&lt;div&gt;&lt;br&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;That was very, very, very unexpected. Nothing against it. It is lovely. But I have the feeling most Historical Fiction books I've been reading lately are all homosexual couples... I kind of like daydreaming with straights... since I am... happy for the characters but leaves me with no daydreaming topic hahaha&lt;/span&gt;&lt;/div&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;It starts slooowww, the whole first part is the MC in the maternity room. The dialog style is annoying. I keep having to go back to reread it after I know who spoke and if out loud or in thoughts.&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;&lt;br&gt;&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;The concept itself makes me keep reading to see where it goes.&lt;/span&gt;&lt;/div&gt;&lt;/div&gt;&lt;div&gt;&lt;br&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;Nop. not going to finish it. It is so much science and so little story... I am sure that without the science, it would have been one of his many short stories.&lt;/span&gt;&lt;/div&gt;&lt;/div&gt;&lt;div&gt;&lt;br&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;Got too technical and no plot... I could not read naother word about the secret weapons program.&lt;/span&gt;&lt;/div&gt;&lt;/div&gt;&lt;div&gt;&lt;br&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;Wow. Loved the narration. Was sad for some characters, :( was sad for humanity. There is something about end of times books that just triggers me to embrace this moment because one day we will be gone.&lt;/span&gt;&lt;/div&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;Entertaining but not amazing. Like TV in a tired night.&lt;/span&gt;&lt;/div&gt;&lt;/div&gt;&lt;div&gt;&lt;br&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;It's getting a bit better.&lt;/span&gt;&lt;/div&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;span style="font-size: 12px;"&gt;It is sooo weird and condescending with criticizing every single element of modern society. Even things that should be logical. If they study life on other planets, they should know all life is different. This shows the "aliens" as stupid ATM... and that annoys me. But I am intrigued. The writing is good. It is just the character... so annoying.&lt;/span&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;The main character is annoying. The whole way. We should count how many times the word Asshole appears in the book.&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;What kept me reading is the theme.&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;A lot of things seem to happen at random, so much in one go, but it is entertaining. It plays like&amp;nbsp; a movie in my head. Or a miniseries considering the length.&lt;/span&gt;&lt;/div&gt;&lt;div&gt;&lt;span style="font-size: 12px;"&gt;What a crazy rideeeeeeeee&lt;/span&gt;&lt;/div&gt;&lt;/div&gt;&lt;div&gt;&lt;br&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>😮</t>
+  </si>
+  <si>
+    <t>😑</t>
+  </si>
+  <si>
+    <t>❌</t>
   </si>
 </sst>
 </file>
@@ -956,9 +952,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="171" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1113,8 +1109,20 @@
       <name val="Lato"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF212529"/>
+      <name val="Quicksand"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1306,6 +1314,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -1483,7 +1497,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1496,11 +1510,24 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="19" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1863,12 +1890,12 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>125</v>
       </c>
@@ -1876,7 +1903,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1884,7 +1911,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1892,7 +1919,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1900,7 +1927,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1908,7 +1935,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1916,7 +1943,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1924,7 +1951,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1932,7 +1959,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1940,7 +1967,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1948,7 +1975,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1956,7 +1983,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1977,21 +2004,21 @@
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="30" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.54296875" customWidth="1"/>
+    <col min="4" max="4" width="21.54296875" customWidth="1"/>
+    <col min="5" max="5" width="6.1796875" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.453125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>127</v>
       </c>
@@ -2023,7 +2050,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2052,7 +2079,7 @@
         <v>44607</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2081,7 +2108,7 @@
         <v>44638</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2107,7 +2134,7 @@
         <v>44611</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2136,7 +2163,7 @@
         <v>44631</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2165,7 +2192,7 @@
         <v>44646</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2194,7 +2221,7 @@
         <v>44628</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2223,7 +2250,7 @@
         <v>44616</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2252,7 +2279,7 @@
         <v>44608</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2281,7 +2308,7 @@
         <v>44347</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2310,7 +2337,7 @@
         <v>44216</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2339,7 +2366,7 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2368,7 +2395,7 @@
         <v>44415</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2397,7 +2424,7 @@
         <v>44414</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2426,7 +2453,7 @@
         <v>44431</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2455,7 +2482,7 @@
         <v>44496</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2484,7 +2511,7 @@
         <v>44485</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2513,7 +2540,7 @@
         <v>44474</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2542,7 +2569,7 @@
         <v>44602</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2571,7 +2598,7 @@
         <v>44581</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2600,7 +2627,7 @@
         <v>43896</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2629,7 +2656,7 @@
         <v>43934</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2658,7 +2685,7 @@
         <v>43946</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2687,7 +2714,7 @@
         <v>43948</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2716,7 +2743,7 @@
         <v>43940</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2745,7 +2772,7 @@
         <v>43956</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2774,7 +2801,7 @@
         <v>43953</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2803,7 +2830,7 @@
         <v>43965</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2832,7 +2859,7 @@
         <v>43967</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2861,7 +2888,7 @@
         <v>43970</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2887,7 +2914,7 @@
         <v>43971</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2916,7 +2943,7 @@
         <v>43979</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2945,7 +2972,7 @@
         <v>43991</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2974,7 +3001,7 @@
         <v>43991</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3003,7 +3030,7 @@
         <v>43985</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3032,7 +3059,7 @@
         <v>44003</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3061,7 +3088,7 @@
         <v>44023</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3090,7 +3117,7 @@
         <v>44029</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3119,7 +3146,7 @@
         <v>44054</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3148,7 +3175,7 @@
         <v>44076</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3177,7 +3204,7 @@
         <v>44610</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3206,7 +3233,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3235,7 +3262,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3264,7 +3291,7 @@
         <v>44559</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3293,7 +3320,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3322,7 +3349,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3351,7 +3378,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3380,7 +3407,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3409,7 +3436,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3438,7 +3465,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>51</v>
       </c>
@@ -3467,7 +3494,7 @@
         <v>44641</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>52</v>
       </c>
@@ -3496,7 +3523,7 @@
         <v>44648</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>53</v>
       </c>
@@ -3525,7 +3552,7 @@
         <v>44652</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>54</v>
       </c>
@@ -3554,7 +3581,7 @@
         <v>44654</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>55</v>
       </c>
@@ -3583,7 +3610,7 @@
         <v>44666</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>56</v>
       </c>
@@ -3612,7 +3639,7 @@
         <v>44660</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>57</v>
       </c>
@@ -3641,7 +3668,7 @@
         <v>44667</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>58</v>
       </c>
@@ -3670,7 +3697,7 @@
         <v>44670</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>59</v>
       </c>
@@ -3699,7 +3726,7 @@
         <v>44674</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>60</v>
       </c>
@@ -3728,7 +3755,7 @@
         <v>44686</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>61</v>
       </c>
@@ -3757,7 +3784,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>62</v>
       </c>
@@ -3786,7 +3813,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>63</v>
       </c>
@@ -3815,7 +3842,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>64</v>
       </c>
@@ -3844,7 +3871,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>65</v>
       </c>
@@ -3873,7 +3900,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>66</v>
       </c>
@@ -3902,7 +3929,7 @@
         <v>44697</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>67</v>
       </c>
@@ -3931,7 +3958,7 @@
         <v>44742</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>68</v>
       </c>
@@ -3983,21 +4010,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="44.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="44.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="95.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="95.26953125" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>127</v>
       </c>
@@ -4017,295 +4044,301 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:6" s="10" customFormat="1" ht="290.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="C2" s="12">
+        <v>44607</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="C2" s="7">
-        <v>44607</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" s="10">
+        <v>352</v>
+      </c>
+      <c r="F2" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="C3" s="13">
+        <v>44633</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="E3" s="10">
+        <v>36</v>
+      </c>
+      <c r="F3" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="C4" s="13">
+        <v>44635</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="E4" s="10">
+        <v>58</v>
+      </c>
+      <c r="F4" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="C5" s="13">
+        <v>44637</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="E2">
-        <v>352</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="E5" s="10">
+        <v>142</v>
+      </c>
+      <c r="F5" s="10">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>229</v>
-      </c>
-      <c r="C3" s="6">
-        <v>44633</v>
-      </c>
-      <c r="E3">
-        <v>36</v>
-      </c>
-      <c r="F3">
+    </row>
+    <row r="6" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="C6" s="13">
+        <v>44637</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="E6" s="10">
+        <v>209</v>
+      </c>
+      <c r="F6" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="7" spans="1:6" s="10" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="10">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="C7" s="13">
+        <v>44638</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="E7" s="10">
+        <v>232</v>
+      </c>
+      <c r="F7" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="10" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="10">
+        <v>8</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="C8" s="13">
+        <v>44638</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="E8" s="10">
+        <v>288</v>
+      </c>
+      <c r="F8" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="10" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="B9" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="C9" s="13">
+        <v>44613</v>
+      </c>
+      <c r="F9" s="10">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>230</v>
-      </c>
-      <c r="C4" s="6">
+    </row>
+    <row r="10" spans="1:6" s="10" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B10" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="C10" s="13">
+        <v>44614</v>
+      </c>
+      <c r="F10" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B11" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="C11" s="13">
+        <v>44615</v>
+      </c>
+      <c r="E11" s="10">
+        <v>64</v>
+      </c>
+      <c r="F11" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="10" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B12" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="C12" s="13">
+        <v>44632</v>
+      </c>
+      <c r="E12" s="10">
+        <v>73</v>
+      </c>
+      <c r="F12" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="10" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B13" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="C13" s="13">
+        <v>44763</v>
+      </c>
+      <c r="E13" s="10">
+        <v>215</v>
+      </c>
+      <c r="F13" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="10" customFormat="1" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="C14" s="13">
+        <v>44767</v>
+      </c>
+      <c r="E14" s="10">
+        <v>240</v>
+      </c>
+      <c r="F14" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="10" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="C15" s="13">
+        <v>44628</v>
+      </c>
+      <c r="F15" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="10" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="C16" s="13">
+        <v>44631</v>
+      </c>
+      <c r="E16" s="10">
+        <v>295</v>
+      </c>
+      <c r="F16" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" s="10" customFormat="1" ht="48.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="15" t="s">
+        <v>290</v>
+      </c>
+      <c r="C17" s="13">
+        <v>44628</v>
+      </c>
+      <c r="F17" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" s="10" customFormat="1" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="C18" s="13">
         <v>44635</v>
       </c>
-      <c r="E4">
-        <v>58</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>226</v>
-      </c>
-      <c r="C5" s="6">
-        <v>44637</v>
-      </c>
-      <c r="D5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E5">
-        <v>142</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="E18" s="10">
+        <v>167</v>
+      </c>
+      <c r="F18" s="10">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>231</v>
-      </c>
-      <c r="C6" s="6">
-        <v>44637</v>
-      </c>
-      <c r="E6">
-        <v>209</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="19" spans="2:6" s="10" customFormat="1" ht="32.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="C19" s="13">
+        <v>44646</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="C7" s="6">
-        <v>44638</v>
-      </c>
-      <c r="D7" t="s">
-        <v>224</v>
-      </c>
-      <c r="E7">
-        <v>232</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>232</v>
-      </c>
-      <c r="C8" s="6">
-        <v>44638</v>
-      </c>
-      <c r="D8" t="s">
-        <v>228</v>
-      </c>
-      <c r="E8">
-        <v>288</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="C9" s="6">
-        <v>44638</v>
-      </c>
-      <c r="D9" t="s">
-        <v>228</v>
-      </c>
-      <c r="E9">
-        <v>288</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="C10" s="6">
-        <v>44613</v>
-      </c>
-      <c r="F10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="C11" s="6">
-        <v>44614</v>
-      </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C12" s="6">
-        <v>44615</v>
-      </c>
-      <c r="E12">
-        <v>64</v>
-      </c>
-      <c r="F12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="C13" s="6">
-        <v>44632</v>
-      </c>
-      <c r="E13">
-        <v>73</v>
-      </c>
-      <c r="F13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C14" s="6">
-        <v>44763</v>
-      </c>
-      <c r="E14">
-        <v>215</v>
-      </c>
-      <c r="F14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C15" s="6">
-        <v>44628</v>
-      </c>
-      <c r="F15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="C16" s="6">
-        <v>44631</v>
-      </c>
-      <c r="E16">
-        <v>295</v>
-      </c>
-      <c r="F16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="C17" s="6">
-        <v>44628</v>
-      </c>
-      <c r="F17">
+      <c r="E19" s="10">
+        <v>304</v>
+      </c>
+      <c r="F19" s="10">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C18" s="6">
-        <v>44635</v>
-      </c>
-      <c r="E18">
-        <v>167</v>
-      </c>
-      <c r="F18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="C19" s="6">
-        <v>44646</v>
-      </c>
-      <c r="D19" t="s">
-        <v>244</v>
-      </c>
-      <c r="E19">
-        <v>304</v>
-      </c>
-      <c r="F19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>245</v>
+    <row r="20" spans="2:6" ht="32.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="8" t="s">
+        <v>299</v>
       </c>
       <c r="C20" s="6">
         <v>44628</v>
       </c>
+      <c r="D20" s="9" t="s">
+        <v>300</v>
+      </c>
       <c r="E20">
         <v>336</v>
       </c>
@@ -4313,13 +4346,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>246</v>
+    <row r="21" spans="2:6" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="8" t="s">
+        <v>298</v>
       </c>
       <c r="C21" s="6">
         <v>44613</v>
       </c>
+      <c r="D21" s="9" t="s">
+        <v>301</v>
+      </c>
       <c r="E21">
         <v>100</v>
       </c>
@@ -4327,13 +4363,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>247</v>
+    <row r="22" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="8" t="s">
+        <v>297</v>
       </c>
       <c r="C22" s="6">
         <v>44615</v>
       </c>
+      <c r="D22" s="9" t="s">
+        <v>301</v>
+      </c>
       <c r="E22">
         <v>150</v>
       </c>
@@ -4341,13 +4380,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
-        <v>248</v>
+    <row r="23" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="8" t="s">
+        <v>296</v>
       </c>
       <c r="C23" s="6">
         <v>44616</v>
       </c>
+      <c r="D23" s="9" t="s">
+        <v>300</v>
+      </c>
       <c r="E23">
         <v>290</v>
       </c>
@@ -4355,13 +4397,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
-        <v>249</v>
+    <row r="24" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="8" t="s">
+        <v>295</v>
       </c>
       <c r="C24" s="6">
         <v>44385</v>
       </c>
+      <c r="D24" s="9" t="s">
+        <v>247</v>
+      </c>
       <c r="E24">
         <v>602</v>
       </c>
@@ -4369,13 +4414,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>250</v>
+    <row r="25" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="8" t="s">
+        <v>294</v>
       </c>
       <c r="C25" s="6">
         <v>44415</v>
       </c>
+      <c r="D25" s="9" t="s">
+        <v>301</v>
+      </c>
       <c r="E25">
         <v>100</v>
       </c>
@@ -4383,13 +4431,16 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
-        <v>251</v>
+    <row r="26" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="8" t="s">
+        <v>293</v>
       </c>
       <c r="C26" s="6">
         <v>44415</v>
       </c>
+      <c r="D26" s="9" t="s">
+        <v>302</v>
+      </c>
       <c r="E26">
         <v>110</v>
       </c>
@@ -4397,9 +4448,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B27" s="1" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="C27" s="6">
         <v>44431</v>
@@ -4411,9 +4462,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B28" s="1" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="C28" s="6">
         <v>44602</v>
@@ -4422,9 +4473,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="8" t="s">
-        <v>254</v>
+    <row r="29" spans="2:6" ht="15" x14ac:dyDescent="0.4">
+      <c r="B29" s="7" t="s">
+        <v>230</v>
       </c>
       <c r="C29" s="6">
         <v>44602</v>
@@ -4436,9 +4487,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B30" s="1" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="C30" s="6">
         <v>44602</v>
@@ -4450,9 +4501,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="C31" s="6">
         <v>44677</v>
@@ -4461,29 +4512,29 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B32" s="1" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
       <c r="C32" s="6">
         <v>44670</v>
       </c>
       <c r="D32" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F32">
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" ht="58" x14ac:dyDescent="0.35">
       <c r="B33" s="1" t="s">
-        <v>258</v>
+        <v>234</v>
       </c>
       <c r="C33" s="6">
         <v>44670</v>
       </c>
       <c r="D33" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E33">
         <v>221</v>
@@ -4492,43 +4543,43 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B34" s="1" t="s">
-        <v>259</v>
+        <v>235</v>
       </c>
       <c r="C34" s="6">
         <v>44670</v>
       </c>
       <c r="D34" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F34">
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B35" s="1" t="s">
-        <v>260</v>
+        <v>236</v>
       </c>
       <c r="C35" s="6">
         <v>44670</v>
       </c>
       <c r="D35" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F35">
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B36" s="1" t="s">
-        <v>262</v>
+        <v>238</v>
       </c>
       <c r="C36" s="6">
         <v>44664</v>
       </c>
       <c r="D36" t="s">
-        <v>267</v>
+        <v>243</v>
       </c>
       <c r="E36">
         <v>100</v>
@@ -4537,15 +4588,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B37" s="1" t="s">
-        <v>261</v>
+        <v>237</v>
       </c>
       <c r="C37" s="6">
         <v>44661</v>
       </c>
       <c r="D37" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="E37">
         <v>18</v>
@@ -4554,15 +4605,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B38" s="1" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
       <c r="C38" s="6">
         <v>44664</v>
       </c>
       <c r="D38" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E38">
         <v>182</v>
@@ -4571,15 +4622,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B39" s="1" t="s">
-        <v>264</v>
+        <v>240</v>
       </c>
       <c r="C39" s="6">
         <v>44664</v>
       </c>
       <c r="D39" t="s">
-        <v>269</v>
+        <v>245</v>
       </c>
       <c r="E39">
         <v>235</v>
@@ -4588,15 +4639,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B40" s="1" t="s">
-        <v>265</v>
+        <v>241</v>
       </c>
       <c r="C40" s="6">
         <v>44666</v>
       </c>
       <c r="D40" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
       <c r="E40">
         <v>325</v>
@@ -4605,15 +4656,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B41" s="1" t="s">
-        <v>266</v>
+        <v>242</v>
       </c>
       <c r="C41" s="6">
         <v>44667</v>
       </c>
       <c r="D41" t="s">
-        <v>271</v>
+        <v>247</v>
       </c>
       <c r="E41">
         <v>476</v>
@@ -4622,15 +4673,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B42" s="1" t="s">
-        <v>272</v>
+        <v>248</v>
       </c>
       <c r="C42" s="6">
         <v>44660</v>
       </c>
       <c r="D42" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
       <c r="E42">
         <v>389</v>
@@ -4639,9 +4690,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B43" s="1" t="s">
-        <v>273</v>
+        <v>249</v>
       </c>
       <c r="C43" s="6">
         <v>44649</v>
@@ -4653,9 +4704,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B44" s="1" t="s">
-        <v>275</v>
+        <v>251</v>
       </c>
       <c r="C44" s="6">
         <v>44649</v>
@@ -4667,9 +4718,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B45" s="1" t="s">
-        <v>274</v>
+        <v>250</v>
       </c>
       <c r="C45" s="6">
         <v>44649</v>
@@ -4681,9 +4732,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B46" s="1" t="s">
-        <v>276</v>
+        <v>252</v>
       </c>
       <c r="C46" s="6">
         <v>44649</v>
@@ -4695,9 +4746,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:6" ht="87" x14ac:dyDescent="0.35">
       <c r="B47" s="1" t="s">
-        <v>277</v>
+        <v>253</v>
       </c>
       <c r="C47" s="6">
         <v>44649</v>
@@ -4709,9 +4760,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:6" ht="87" x14ac:dyDescent="0.35">
       <c r="B48" s="1" t="s">
-        <v>277</v>
+        <v>253</v>
       </c>
       <c r="C48" s="6">
         <v>44649</v>
@@ -4723,9 +4774,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:6" ht="87" x14ac:dyDescent="0.35">
       <c r="B49" s="1" t="s">
-        <v>278</v>
+        <v>254</v>
       </c>
       <c r="C49" s="6">
         <v>44649</v>
@@ -4737,9 +4788,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B50" s="1" t="s">
-        <v>279</v>
+        <v>255</v>
       </c>
       <c r="C50" s="6">
         <v>44650</v>
@@ -4748,9 +4799,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B51" s="1" t="s">
-        <v>280</v>
+        <v>256</v>
       </c>
       <c r="C51" s="6">
         <v>44650</v>
@@ -4759,9 +4810,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B52" s="1" t="s">
-        <v>281</v>
+        <v>257</v>
       </c>
       <c r="C52" s="6">
         <v>44650</v>
@@ -4770,9 +4821,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B53" s="1" t="s">
-        <v>282</v>
+        <v>258</v>
       </c>
       <c r="C53" s="6">
         <v>44650</v>
@@ -4784,9 +4835,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B54" s="1" t="s">
-        <v>283</v>
+        <v>259</v>
       </c>
       <c r="C54" s="6">
         <v>44651</v>
@@ -4798,9 +4849,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B55" s="1" t="s">
-        <v>284</v>
+        <v>260</v>
       </c>
       <c r="C55" s="6">
         <v>44651</v>
@@ -4812,9 +4863,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B56" s="1" t="s">
-        <v>285</v>
+        <v>261</v>
       </c>
       <c r="C56" s="6">
         <v>44651</v>
@@ -4826,9 +4877,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B57" s="1" t="s">
-        <v>286</v>
+        <v>262</v>
       </c>
       <c r="C57" s="6">
         <v>44652</v>
@@ -4840,9 +4891,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B58" s="1" t="s">
-        <v>287</v>
+        <v>263</v>
       </c>
       <c r="C58" s="6">
         <v>44654</v>
@@ -4854,9 +4905,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="2:6" ht="225" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:6" ht="217.5" x14ac:dyDescent="0.35">
       <c r="B59" s="1" t="s">
-        <v>288</v>
+        <v>264</v>
       </c>
       <c r="C59" s="6">
         <v>44654</v>
@@ -4868,9 +4919,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
-        <v>289</v>
+        <v>265</v>
       </c>
       <c r="C60" s="6">
         <v>44647</v>
@@ -4879,9 +4930,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B61" s="1" t="s">
-        <v>290</v>
+        <v>266</v>
       </c>
       <c r="C61" s="6">
         <v>44640</v>
@@ -4893,9 +4944,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="62" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B62" s="1" t="s">
-        <v>291</v>
+        <v>267</v>
       </c>
       <c r="C62" s="6">
         <v>44641</v>
@@ -4907,9 +4958,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="63" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B63" s="1" t="s">
-        <v>292</v>
+        <v>268</v>
       </c>
       <c r="C63" s="6">
         <v>44643</v>
@@ -4921,9 +4972,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B64" s="1" t="s">
-        <v>293</v>
+        <v>269</v>
       </c>
       <c r="C64" s="6">
         <v>44646</v>
@@ -4935,9 +4986,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B65" s="1" t="s">
-        <v>294</v>
+        <v>270</v>
       </c>
       <c r="C65" s="6">
         <v>44647</v>
@@ -4949,9 +5000,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="66" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B66" s="1" t="s">
-        <v>295</v>
+        <v>271</v>
       </c>
       <c r="C66" s="6">
         <v>44648</v>
@@ -4963,9 +5014,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="67" spans="2:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:6" ht="101.5" x14ac:dyDescent="0.35">
       <c r="B67" s="1" t="s">
-        <v>296</v>
+        <v>272</v>
       </c>
       <c r="C67" s="6">
         <v>44648</v>
@@ -4977,9 +5028,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B68" s="1" t="s">
-        <v>297</v>
+        <v>273</v>
       </c>
       <c r="C68" s="6">
         <v>44641</v>
@@ -5013,9 +5064,9 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>143</v>
       </c>
@@ -5023,7 +5074,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5031,7 +5082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5039,7 +5090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -5047,7 +5098,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -5055,7 +5106,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -5063,7 +5114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -5071,7 +5122,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>5</v>
       </c>
@@ -5079,7 +5130,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>6</v>
       </c>
@@ -5087,7 +5138,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>7</v>
       </c>
@@ -5095,7 +5146,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>8</v>
       </c>
@@ -5103,7 +5154,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>9</v>
       </c>
@@ -5111,7 +5162,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>10</v>
       </c>
@@ -5119,7 +5170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>11</v>
       </c>
@@ -5127,7 +5178,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>12</v>
       </c>
@@ -5135,7 +5186,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>13</v>
       </c>
@@ -5143,7 +5194,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>14</v>
       </c>
@@ -5151,7 +5202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>15</v>
       </c>
@@ -5159,7 +5210,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>16</v>
       </c>
@@ -5167,7 +5218,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>17</v>
       </c>
@@ -5175,7 +5226,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>18</v>
       </c>
@@ -5183,7 +5234,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>19</v>
       </c>
@@ -5191,7 +5242,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>20</v>
       </c>
@@ -5199,7 +5250,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>21</v>
       </c>
@@ -5207,7 +5258,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>22</v>
       </c>
@@ -5215,7 +5266,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>23</v>
       </c>
@@ -5223,7 +5274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>24</v>
       </c>
@@ -5231,7 +5282,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>25</v>
       </c>
@@ -5239,7 +5290,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>26</v>
       </c>
@@ -5247,7 +5298,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>27</v>
       </c>
@@ -5255,7 +5306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>28</v>
       </c>
@@ -5263,7 +5314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>29</v>
       </c>
@@ -5271,7 +5322,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>30</v>
       </c>
@@ -5279,7 +5330,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>31</v>
       </c>
@@ -5287,7 +5338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>32</v>
       </c>
@@ -5295,7 +5346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>33</v>
       </c>
@@ -5303,7 +5354,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>34</v>
       </c>
@@ -5311,7 +5362,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>35</v>
       </c>
@@ -5319,7 +5370,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>36</v>
       </c>
@@ -5327,7 +5378,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>37</v>
       </c>
@@ -5335,7 +5386,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>38</v>
       </c>
@@ -5343,7 +5394,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>39</v>
       </c>
@@ -5351,7 +5402,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>40</v>
       </c>
@@ -5359,7 +5410,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>41</v>
       </c>
@@ -5367,7 +5418,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>42</v>
       </c>
@@ -5375,7 +5426,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>43</v>
       </c>
@@ -5383,7 +5434,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>44</v>
       </c>
@@ -5391,7 +5442,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>45</v>
       </c>
@@ -5399,7 +5450,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>46</v>
       </c>
@@ -5407,7 +5458,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>47</v>
       </c>
@@ -5415,7 +5466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>47</v>
       </c>
@@ -5423,7 +5474,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>48</v>
       </c>
@@ -5431,7 +5482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>49</v>
       </c>
@@ -5439,7 +5490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>51</v>
       </c>
@@ -5447,7 +5498,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>52</v>
       </c>
@@ -5455,7 +5506,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>53</v>
       </c>
@@ -5463,7 +5514,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>54</v>
       </c>
@@ -5471,7 +5522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>54</v>
       </c>
@@ -5479,7 +5530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>55</v>
       </c>
@@ -5487,7 +5538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>56</v>
       </c>
@@ -5495,7 +5546,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>57</v>
       </c>
@@ -5503,7 +5554,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>58</v>
       </c>
@@ -5511,7 +5562,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>59</v>
       </c>
@@ -5519,7 +5570,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>60</v>
       </c>
@@ -5527,7 +5578,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>61</v>
       </c>
@@ -5535,7 +5586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>62</v>
       </c>
@@ -5543,7 +5594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>63</v>
       </c>
@@ -5551,7 +5602,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>64</v>
       </c>
@@ -5559,7 +5610,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>65</v>
       </c>
@@ -5567,7 +5618,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>66</v>
       </c>
@@ -5575,7 +5626,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>67</v>
       </c>
@@ -5583,7 +5634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
organized and cleaned mappings :) /books /shelves /logs
</commit_message>
<xml_diff>
--- a/mylibrary.xlsx
+++ b/mylibrary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\munozm\Desktop\imreading\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B297729-0633-4A59-9C34-5CA69CC3F702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B291AD2-17E4-41BF-A969-2A196EAE15DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2280" yWindow="2280" windowWidth="25800" windowHeight="10140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1122,7 +1122,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1310,12 +1310,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1497,7 +1491,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1512,20 +1506,16 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4010,8 +4000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B34" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4044,407 +4034,407 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="10" customFormat="1" ht="290.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="10">
+    <row r="2" spans="1:6" s="8" customFormat="1" ht="290.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="10">
         <v>44607</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="8">
         <v>352</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="10">
+    <row r="3" spans="1:6" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="11">
         <v>44633</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="8">
         <v>36</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="10">
+    <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="11">
         <v>44635</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="8">
         <v>58</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="10">
+    <row r="5" spans="1:6" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="11">
         <v>44637</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="8">
         <v>142</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="10">
+    <row r="6" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="11">
         <v>44637</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="8">
         <v>209</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="10" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="10">
+    <row r="7" spans="1:6" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="11">
         <v>44638</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="8">
         <v>232</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="10" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="10">
+    <row r="8" spans="1:6" s="8" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="8">
         <v>8</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="11">
         <v>44638</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="8">
         <v>288</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="10" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="B9" s="11" t="s">
+    <row r="9" spans="1:6" s="8" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="B9" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="11">
         <v>44613</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="10" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B10" s="11" t="s">
+    <row r="10" spans="1:6" s="8" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B10" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="11">
         <v>44614</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="B11" s="11" t="s">
+    <row r="11" spans="1:6" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B11" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="11">
         <v>44615</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="8">
         <v>64</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="10" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B12" s="11" t="s">
+    <row r="12" spans="1:6" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B12" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="11">
         <v>44632</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="8">
         <v>73</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="10" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B13" s="11" t="s">
+    <row r="13" spans="1:6" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B13" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="11">
         <v>44763</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="8">
         <v>215</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="10" customFormat="1" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="11" t="s">
+    <row r="14" spans="1:6" s="8" customFormat="1" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="11">
         <v>44767</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="8">
         <v>240</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="10" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="15" t="s">
+    <row r="15" spans="1:6" s="8" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="13" t="s">
         <v>292</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="11">
         <v>44628</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="10" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="15" t="s">
+    <row r="16" spans="1:6" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="11">
         <v>44631</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="8">
         <v>295</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:6" s="10" customFormat="1" ht="48.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="15" t="s">
+    <row r="17" spans="2:6" s="8" customFormat="1" ht="48.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="13" t="s">
         <v>290</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="11">
         <v>44628</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:6" s="10" customFormat="1" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="11" t="s">
+    <row r="18" spans="2:6" s="8" customFormat="1" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="11">
         <v>44635</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="8">
         <v>167</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:6" s="10" customFormat="1" ht="32.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="15" t="s">
+    <row r="19" spans="2:6" s="8" customFormat="1" ht="32.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="11">
         <v>44646</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="8">
         <v>304</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="32.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="8" t="s">
+    <row r="20" spans="2:6" s="8" customFormat="1" ht="32.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="11">
         <v>44628</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="12" t="s">
         <v>300</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="8">
         <v>336</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="8">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="8" t="s">
+    <row r="21" spans="2:6" s="8" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="13" t="s">
         <v>298</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="11">
         <v>44613</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="12" t="s">
         <v>301</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="8">
         <v>100</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="8">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="8" t="s">
+    <row r="22" spans="2:6" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="13" t="s">
         <v>297</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="11">
         <v>44615</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="12" t="s">
         <v>301</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="8">
         <v>150</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="8">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="8" t="s">
+    <row r="23" spans="2:6" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="13" t="s">
         <v>296</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="11">
         <v>44616</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="12" t="s">
         <v>300</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="8">
         <v>290</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="8">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="8" t="s">
+    <row r="24" spans="2:6" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="11">
         <v>44385</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="8">
         <v>602</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="8">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="8" t="s">
+    <row r="25" spans="2:6" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="11">
         <v>44415</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="12" t="s">
         <v>301</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="8">
         <v>100</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="8">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="8" t="s">
+    <row r="26" spans="2:6" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="13" t="s">
         <v>293</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="11">
         <v>44415</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="12" t="s">
         <v>302</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="8">
         <v>110</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="8">
         <v>13</v>
       </c>
     </row>

</xml_diff>